<commit_message>
update of recreated data files
corrects missing subject data
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -161,10 +161,10 @@
     <t>peripheral blood mononuclear cell</t>
   </si>
   <si>
-    <t>serum</t>
-  </si>
-  <si>
-    <t>body skin</t>
+    <t>blood serum</t>
+  </si>
+  <si>
+    <t>skin of body</t>
   </si>
   <si>
     <t>label</t>
@@ -22930,7 +22930,7 @@
         <v>411</v>
       </c>
       <c r="P172" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q172" t="s">
         <v>451</v>
@@ -23043,7 +23043,7 @@
         <v>411</v>
       </c>
       <c r="P173" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q173" t="s">
         <v>451</v>
@@ -23156,7 +23156,7 @@
         <v>411</v>
       </c>
       <c r="P174" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q174" t="s">
         <v>451</v>
@@ -23269,7 +23269,7 @@
         <v>411</v>
       </c>
       <c r="P175" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q175" t="s">
         <v>451</v>
@@ -23382,7 +23382,7 @@
         <v>411</v>
       </c>
       <c r="P176" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q176" t="s">
         <v>451</v>
@@ -23495,7 +23495,7 @@
         <v>411</v>
       </c>
       <c r="P177" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q177" t="s">
         <v>451</v>
@@ -23608,7 +23608,7 @@
         <v>411</v>
       </c>
       <c r="P178" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q178" t="s">
         <v>451</v>
@@ -23721,7 +23721,7 @@
         <v>411</v>
       </c>
       <c r="P179" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q179" t="s">
         <v>451</v>
@@ -23834,7 +23834,7 @@
         <v>411</v>
       </c>
       <c r="P180" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q180" t="s">
         <v>451</v>
@@ -23947,7 +23947,7 @@
         <v>411</v>
       </c>
       <c r="P181" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q181" t="s">
         <v>451</v>
@@ -24060,7 +24060,7 @@
         <v>411</v>
       </c>
       <c r="P182" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q182" t="s">
         <v>451</v>
@@ -24173,7 +24173,7 @@
         <v>411</v>
       </c>
       <c r="P183" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q183" t="s">
         <v>451</v>
@@ -24286,7 +24286,7 @@
         <v>411</v>
       </c>
       <c r="P184" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q184" t="s">
         <v>451</v>
@@ -24399,7 +24399,7 @@
         <v>411</v>
       </c>
       <c r="P185" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q185" t="s">
         <v>451</v>
@@ -24512,7 +24512,7 @@
         <v>411</v>
       </c>
       <c r="P186" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q186" t="s">
         <v>451</v>
@@ -24625,7 +24625,7 @@
         <v>411</v>
       </c>
       <c r="P187" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q187" t="s">
         <v>451</v>
@@ -24738,7 +24738,7 @@
         <v>411</v>
       </c>
       <c r="P188" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q188" t="s">
         <v>451</v>
@@ -24851,7 +24851,7 @@
         <v>411</v>
       </c>
       <c r="P189" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q189" t="s">
         <v>451</v>
@@ -24964,7 +24964,7 @@
         <v>411</v>
       </c>
       <c r="P190" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q190" t="s">
         <v>451</v>
@@ -25077,7 +25077,7 @@
         <v>411</v>
       </c>
       <c r="P191" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q191" t="s">
         <v>450</v>
@@ -25190,7 +25190,7 @@
         <v>411</v>
       </c>
       <c r="P192" t="s">
-        <v>417</v>
+        <v>43</v>
       </c>
       <c r="Q192" t="s">
         <v>450</v>

</xml_diff>

<commit_message>
updated files from unifying influenza handling
updated files from unifying influenza handling
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -1250,9 +1250,6 @@
     <t>influenza A virus (A/California/7/2009(H1N1))</t>
   </si>
   <si>
-    <t>influenza A virus (H1N1)</t>
-  </si>
-  <si>
     <t>vaccine year</t>
   </si>
   <si>
@@ -1268,6 +1265,9 @@
     <t>2010</t>
   </si>
   <si>
+    <t>2009, pan</t>
+  </si>
+  <si>
     <t>2007, 2008, 2009</t>
   </si>
   <si>
@@ -1277,6 +1277,9 @@
     <t>2009mv</t>
   </si>
   <si>
+    <t>pan</t>
+  </si>
+  <si>
     <t>exposure material (name)</t>
   </si>
   <si>
@@ -1365,9 +1368,6 @@
   </si>
   <si>
     <t>Pandemrix</t>
-  </si>
-  <si>
-    <t>Pandemrix (A/California/7/09 (H1N1))</t>
   </si>
   <si>
     <t>vaccine</t>
@@ -4285,10 +4285,10 @@
         <v>394</v>
       </c>
       <c r="P7" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="Q7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="R7" t="s">
         <v>453</v>
@@ -4401,7 +4401,7 @@
         <v>43</v>
       </c>
       <c r="Q8" t="s">
-        <v>422</v>
+        <v>423</v>
       </c>
       <c r="R8" t="s">
         <v>454</v>
@@ -4514,7 +4514,7 @@
         <v>43</v>
       </c>
       <c r="Q9" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="R9" t="s">
         <v>455</v>
@@ -4627,7 +4627,7 @@
         <v>43</v>
       </c>
       <c r="Q10" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="R10" t="s">
         <v>455</v>
@@ -4740,7 +4740,7 @@
         <v>43</v>
       </c>
       <c r="Q11" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="R11" t="s">
         <v>456</v>
@@ -4853,7 +4853,7 @@
         <v>43</v>
       </c>
       <c r="Q12" t="s">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="R12" t="s">
         <v>455</v>
@@ -4963,10 +4963,10 @@
         <v>396</v>
       </c>
       <c r="P13" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q13" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R13" t="s">
         <v>457</v>
@@ -5076,10 +5076,10 @@
         <v>396</v>
       </c>
       <c r="P14" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q14" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R14" t="s">
         <v>457</v>
@@ -5189,10 +5189,10 @@
         <v>396</v>
       </c>
       <c r="P15" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q15" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R15" t="s">
         <v>457</v>
@@ -5302,10 +5302,10 @@
         <v>396</v>
       </c>
       <c r="P16" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q16" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R16" t="s">
         <v>457</v>
@@ -5415,10 +5415,10 @@
         <v>396</v>
       </c>
       <c r="P17" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q17" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R17" t="s">
         <v>457</v>
@@ -5528,10 +5528,10 @@
         <v>396</v>
       </c>
       <c r="P18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q18" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R18" t="s">
         <v>457</v>
@@ -5644,7 +5644,7 @@
         <v>43</v>
       </c>
       <c r="Q19" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="R19" t="s">
         <v>458</v>
@@ -5757,7 +5757,7 @@
         <v>43</v>
       </c>
       <c r="Q20" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="R20" t="s">
         <v>458</v>
@@ -5867,10 +5867,10 @@
         <v>398</v>
       </c>
       <c r="P21" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Q21" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R21" t="s">
         <v>457</v>
@@ -5983,7 +5983,7 @@
         <v>43</v>
       </c>
       <c r="Q22" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R22" t="s">
         <v>459</v>
@@ -6096,7 +6096,7 @@
         <v>43</v>
       </c>
       <c r="Q23" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R23" t="s">
         <v>459</v>
@@ -6209,7 +6209,7 @@
         <v>43</v>
       </c>
       <c r="Q24" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R24" t="s">
         <v>459</v>
@@ -6322,7 +6322,7 @@
         <v>43</v>
       </c>
       <c r="Q25" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R25" t="s">
         <v>459</v>
@@ -6432,10 +6432,10 @@
         <v>400</v>
       </c>
       <c r="P26" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q26" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="R26" t="s">
         <v>460</v>
@@ -6545,10 +6545,10 @@
         <v>400</v>
       </c>
       <c r="P27" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q27" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="R27" t="s">
         <v>461</v>
@@ -6658,10 +6658,10 @@
         <v>400</v>
       </c>
       <c r="P28" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q28" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="R28" t="s">
         <v>461</v>
@@ -6774,7 +6774,7 @@
         <v>43</v>
       </c>
       <c r="Q29" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R29" t="s">
         <v>462</v>
@@ -6798,7 +6798,7 @@
         <v>587</v>
       </c>
       <c r="Y29" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z29" t="s">
         <v>633</v>
@@ -6887,7 +6887,7 @@
         <v>43</v>
       </c>
       <c r="Q30" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R30" t="s">
         <v>462</v>
@@ -6911,7 +6911,7 @@
         <v>587</v>
       </c>
       <c r="Y30" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z30" t="s">
         <v>633</v>
@@ -7000,7 +7000,7 @@
         <v>43</v>
       </c>
       <c r="Q31" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R31" t="s">
         <v>462</v>
@@ -7024,7 +7024,7 @@
         <v>587</v>
       </c>
       <c r="Y31" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z31" t="s">
         <v>633</v>
@@ -7113,7 +7113,7 @@
         <v>43</v>
       </c>
       <c r="Q32" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="R32" t="s">
         <v>462</v>
@@ -7137,7 +7137,7 @@
         <v>587</v>
       </c>
       <c r="Y32" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Z32" t="s">
         <v>633</v>
@@ -7226,7 +7226,7 @@
         <v>43</v>
       </c>
       <c r="Q33" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="R33" t="s">
         <v>463</v>
@@ -7339,7 +7339,7 @@
         <v>43</v>
       </c>
       <c r="Q34" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="R34" t="s">
         <v>464</v>
@@ -7452,7 +7452,7 @@
         <v>43</v>
       </c>
       <c r="Q35" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R35" t="s">
         <v>465</v>
@@ -7565,7 +7565,7 @@
         <v>43</v>
       </c>
       <c r="Q36" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R36" t="s">
         <v>465</v>
@@ -7678,7 +7678,7 @@
         <v>43</v>
       </c>
       <c r="Q37" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R37" t="s">
         <v>465</v>
@@ -7791,7 +7791,7 @@
         <v>43</v>
       </c>
       <c r="Q38" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R38" t="s">
         <v>465</v>
@@ -7904,7 +7904,7 @@
         <v>43</v>
       </c>
       <c r="Q39" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R39" t="s">
         <v>465</v>
@@ -8017,7 +8017,7 @@
         <v>43</v>
       </c>
       <c r="Q40" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R40" t="s">
         <v>465</v>
@@ -8130,7 +8130,7 @@
         <v>43</v>
       </c>
       <c r="Q41" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="R41" t="s">
         <v>466</v>
@@ -8243,7 +8243,7 @@
         <v>43</v>
       </c>
       <c r="Q42" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="R42" t="s">
         <v>467</v>
@@ -8356,7 +8356,7 @@
         <v>43</v>
       </c>
       <c r="Q43" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="R43" t="s">
         <v>467</v>
@@ -8469,7 +8469,7 @@
         <v>43</v>
       </c>
       <c r="Q44" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="R44" t="s">
         <v>467</v>
@@ -8582,7 +8582,7 @@
         <v>43</v>
       </c>
       <c r="Q45" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="R45" t="s">
         <v>468</v>
@@ -8695,7 +8695,7 @@
         <v>43</v>
       </c>
       <c r="Q46" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="R46" t="s">
         <v>469</v>
@@ -8808,7 +8808,7 @@
         <v>43</v>
       </c>
       <c r="Q47" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="R47" t="s">
         <v>469</v>
@@ -8918,10 +8918,10 @@
         <v>406</v>
       </c>
       <c r="P48" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q48" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="R48" t="s">
         <v>470</v>
@@ -9031,10 +9031,10 @@
         <v>407</v>
       </c>
       <c r="P49" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q49" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R49" t="s">
         <v>471</v>
@@ -9144,10 +9144,10 @@
         <v>407</v>
       </c>
       <c r="P50" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q50" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R50" t="s">
         <v>471</v>
@@ -9257,10 +9257,10 @@
         <v>407</v>
       </c>
       <c r="P51" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q51" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R51" t="s">
         <v>471</v>
@@ -9370,10 +9370,10 @@
         <v>407</v>
       </c>
       <c r="P52" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q52" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R52" t="s">
         <v>471</v>
@@ -9483,10 +9483,10 @@
         <v>407</v>
       </c>
       <c r="P53" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q53" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R53" t="s">
         <v>471</v>
@@ -9596,10 +9596,10 @@
         <v>407</v>
       </c>
       <c r="P54" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q54" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R54" t="s">
         <v>471</v>
@@ -9709,10 +9709,10 @@
         <v>407</v>
       </c>
       <c r="P55" t="s">
-        <v>415</v>
+        <v>417</v>
       </c>
       <c r="Q55" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="R55" t="s">
         <v>471</v>
@@ -9825,7 +9825,7 @@
         <v>418</v>
       </c>
       <c r="Q56" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="R56" t="s">
         <v>472</v>
@@ -9938,7 +9938,7 @@
         <v>418</v>
       </c>
       <c r="Q57" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="R57" t="s">
         <v>472</v>
@@ -10051,7 +10051,7 @@
         <v>418</v>
       </c>
       <c r="Q58" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="R58" t="s">
         <v>472</v>
@@ -10164,7 +10164,7 @@
         <v>418</v>
       </c>
       <c r="Q59" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="R59" t="s">
         <v>472</v>
@@ -10274,10 +10274,10 @@
         <v>396</v>
       </c>
       <c r="P60" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="Q60" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="R60" t="s">
         <v>473</v>
@@ -10387,10 +10387,10 @@
         <v>406</v>
       </c>
       <c r="P61" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q61" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R61" t="s">
         <v>457</v>
@@ -10500,10 +10500,10 @@
         <v>406</v>
       </c>
       <c r="P62" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q62" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R62" t="s">
         <v>457</v>
@@ -10613,10 +10613,10 @@
         <v>406</v>
       </c>
       <c r="P63" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q63" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R63" t="s">
         <v>457</v>
@@ -10726,10 +10726,10 @@
         <v>406</v>
       </c>
       <c r="P64" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q64" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R64" t="s">
         <v>457</v>
@@ -10839,10 +10839,10 @@
         <v>406</v>
       </c>
       <c r="P65" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q65" t="s">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="R65" t="s">
         <v>457</v>
@@ -10952,10 +10952,10 @@
         <v>406</v>
       </c>
       <c r="P66" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q66" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="R66" t="s">
         <v>473</v>
@@ -11065,10 +11065,10 @@
         <v>406</v>
       </c>
       <c r="P67" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q67" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R67" t="s">
         <v>474</v>
@@ -11178,10 +11178,10 @@
         <v>406</v>
       </c>
       <c r="P68" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q68" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R68" t="s">
         <v>474</v>
@@ -11291,10 +11291,10 @@
         <v>406</v>
       </c>
       <c r="P69" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q69" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R69" t="s">
         <v>474</v>
@@ -11404,10 +11404,10 @@
         <v>406</v>
       </c>
       <c r="P70" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q70" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R70" t="s">
         <v>474</v>
@@ -11517,10 +11517,10 @@
         <v>406</v>
       </c>
       <c r="P71" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q71" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R71" t="s">
         <v>474</v>
@@ -11630,10 +11630,10 @@
         <v>406</v>
       </c>
       <c r="P72" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q72" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R72" t="s">
         <v>474</v>
@@ -11743,10 +11743,10 @@
         <v>406</v>
       </c>
       <c r="P73" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q73" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R73" t="s">
         <v>474</v>
@@ -11856,10 +11856,10 @@
         <v>406</v>
       </c>
       <c r="P74" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q74" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R74" t="s">
         <v>474</v>
@@ -11969,10 +11969,10 @@
         <v>406</v>
       </c>
       <c r="P75" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q75" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R75" t="s">
         <v>474</v>
@@ -12082,10 +12082,10 @@
         <v>406</v>
       </c>
       <c r="P76" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q76" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R76" t="s">
         <v>474</v>
@@ -12195,10 +12195,10 @@
         <v>406</v>
       </c>
       <c r="P77" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q77" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R77" t="s">
         <v>474</v>
@@ -12308,10 +12308,10 @@
         <v>406</v>
       </c>
       <c r="P78" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q78" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R78" t="s">
         <v>474</v>
@@ -12421,10 +12421,10 @@
         <v>406</v>
       </c>
       <c r="P79" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q79" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R79" t="s">
         <v>474</v>
@@ -12534,10 +12534,10 @@
         <v>406</v>
       </c>
       <c r="P80" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q80" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R80" t="s">
         <v>474</v>
@@ -12647,10 +12647,10 @@
         <v>406</v>
       </c>
       <c r="P81" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q81" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R81" t="s">
         <v>474</v>
@@ -12760,10 +12760,10 @@
         <v>406</v>
       </c>
       <c r="P82" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q82" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R82" t="s">
         <v>474</v>
@@ -12873,10 +12873,10 @@
         <v>406</v>
       </c>
       <c r="P83" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q83" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R83" t="s">
         <v>474</v>
@@ -12986,10 +12986,10 @@
         <v>406</v>
       </c>
       <c r="P84" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q84" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R84" t="s">
         <v>474</v>
@@ -13099,10 +13099,10 @@
         <v>406</v>
       </c>
       <c r="P85" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q85" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R85" t="s">
         <v>474</v>
@@ -13212,10 +13212,10 @@
         <v>406</v>
       </c>
       <c r="P86" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q86" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R86" t="s">
         <v>474</v>
@@ -13325,10 +13325,10 @@
         <v>406</v>
       </c>
       <c r="P87" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q87" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R87" t="s">
         <v>474</v>
@@ -13438,10 +13438,10 @@
         <v>406</v>
       </c>
       <c r="P88" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q88" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R88" t="s">
         <v>474</v>
@@ -13551,10 +13551,10 @@
         <v>406</v>
       </c>
       <c r="P89" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q89" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R89" t="s">
         <v>474</v>
@@ -13664,10 +13664,10 @@
         <v>406</v>
       </c>
       <c r="P90" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q90" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R90" t="s">
         <v>474</v>
@@ -13777,10 +13777,10 @@
         <v>406</v>
       </c>
       <c r="P91" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q91" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R91" t="s">
         <v>474</v>
@@ -13890,10 +13890,10 @@
         <v>406</v>
       </c>
       <c r="P92" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q92" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R92" t="s">
         <v>474</v>
@@ -14003,10 +14003,10 @@
         <v>406</v>
       </c>
       <c r="P93" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q93" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R93" t="s">
         <v>474</v>
@@ -14116,10 +14116,10 @@
         <v>406</v>
       </c>
       <c r="P94" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q94" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R94" t="s">
         <v>474</v>
@@ -14229,10 +14229,10 @@
         <v>406</v>
       </c>
       <c r="P95" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q95" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="R95" t="s">
         <v>474</v>
@@ -14345,7 +14345,7 @@
         <v>43</v>
       </c>
       <c r="Q96" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R96" t="s">
         <v>465</v>
@@ -14458,7 +14458,7 @@
         <v>43</v>
       </c>
       <c r="Q97" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R97" t="s">
         <v>465</v>
@@ -14571,7 +14571,7 @@
         <v>43</v>
       </c>
       <c r="Q98" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R98" t="s">
         <v>465</v>
@@ -14684,7 +14684,7 @@
         <v>43</v>
       </c>
       <c r="Q99" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R99" t="s">
         <v>465</v>
@@ -14797,7 +14797,7 @@
         <v>43</v>
       </c>
       <c r="Q100" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R100" t="s">
         <v>465</v>
@@ -14910,7 +14910,7 @@
         <v>43</v>
       </c>
       <c r="Q101" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="R101" t="s">
         <v>475</v>
@@ -15023,7 +15023,7 @@
         <v>43</v>
       </c>
       <c r="Q102" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="R102" t="s">
         <v>475</v>
@@ -15136,7 +15136,7 @@
         <v>43</v>
       </c>
       <c r="Q103" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R103" t="s">
         <v>476</v>
@@ -15249,7 +15249,7 @@
         <v>43</v>
       </c>
       <c r="Q104" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R104" t="s">
         <v>476</v>
@@ -15362,7 +15362,7 @@
         <v>43</v>
       </c>
       <c r="Q105" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R105" t="s">
         <v>476</v>
@@ -15475,7 +15475,7 @@
         <v>43</v>
       </c>
       <c r="Q106" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R106" t="s">
         <v>476</v>
@@ -15588,7 +15588,7 @@
         <v>43</v>
       </c>
       <c r="Q107" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R107" t="s">
         <v>476</v>
@@ -15701,7 +15701,7 @@
         <v>43</v>
       </c>
       <c r="Q108" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R108" t="s">
         <v>476</v>
@@ -15814,7 +15814,7 @@
         <v>43</v>
       </c>
       <c r="Q109" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R109" t="s">
         <v>476</v>
@@ -15927,7 +15927,7 @@
         <v>43</v>
       </c>
       <c r="Q110" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R110" t="s">
         <v>476</v>
@@ -16040,7 +16040,7 @@
         <v>43</v>
       </c>
       <c r="Q111" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R111" t="s">
         <v>476</v>
@@ -16153,7 +16153,7 @@
         <v>43</v>
       </c>
       <c r="Q112" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R112" t="s">
         <v>476</v>
@@ -16266,7 +16266,7 @@
         <v>43</v>
       </c>
       <c r="Q113" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R113" t="s">
         <v>476</v>
@@ -16379,7 +16379,7 @@
         <v>43</v>
       </c>
       <c r="Q114" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R114" t="s">
         <v>476</v>
@@ -16492,7 +16492,7 @@
         <v>43</v>
       </c>
       <c r="Q115" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R115" t="s">
         <v>476</v>
@@ -16605,7 +16605,7 @@
         <v>43</v>
       </c>
       <c r="Q116" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R116" t="s">
         <v>476</v>
@@ -16718,7 +16718,7 @@
         <v>43</v>
       </c>
       <c r="Q117" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R117" t="s">
         <v>476</v>
@@ -16831,7 +16831,7 @@
         <v>43</v>
       </c>
       <c r="Q118" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R118" t="s">
         <v>476</v>
@@ -16944,7 +16944,7 @@
         <v>43</v>
       </c>
       <c r="Q119" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R119" t="s">
         <v>476</v>
@@ -17057,7 +17057,7 @@
         <v>43</v>
       </c>
       <c r="Q120" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="R120" t="s">
         <v>476</v>
@@ -17167,10 +17167,10 @@
         <v>400</v>
       </c>
       <c r="P121" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q121" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="R121" t="s">
         <v>477</v>
@@ -17280,10 +17280,10 @@
         <v>400</v>
       </c>
       <c r="P122" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="Q122" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="R122" t="s">
         <v>477</v>
@@ -17396,7 +17396,7 @@
         <v>43</v>
       </c>
       <c r="Q123" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R123" t="s">
         <v>476</v>
@@ -17420,7 +17420,7 @@
         <v>605</v>
       </c>
       <c r="Y123" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z123" t="s">
         <v>679</v>
@@ -17509,7 +17509,7 @@
         <v>43</v>
       </c>
       <c r="Q124" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R124" t="s">
         <v>476</v>
@@ -17533,7 +17533,7 @@
         <v>605</v>
       </c>
       <c r="Y124" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z124" t="s">
         <v>679</v>
@@ -17622,7 +17622,7 @@
         <v>43</v>
       </c>
       <c r="Q125" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R125" t="s">
         <v>476</v>
@@ -17646,7 +17646,7 @@
         <v>605</v>
       </c>
       <c r="Y125" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z125" t="s">
         <v>679</v>
@@ -17735,7 +17735,7 @@
         <v>43</v>
       </c>
       <c r="Q126" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R126" t="s">
         <v>476</v>
@@ -17759,7 +17759,7 @@
         <v>605</v>
       </c>
       <c r="Y126" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z126" t="s">
         <v>679</v>
@@ -17848,7 +17848,7 @@
         <v>43</v>
       </c>
       <c r="Q127" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="R127" t="s">
         <v>476</v>
@@ -17872,7 +17872,7 @@
         <v>605</v>
       </c>
       <c r="Y127" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="Z127" t="s">
         <v>679</v>
@@ -17958,10 +17958,10 @@
         <v>406</v>
       </c>
       <c r="P128" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q128" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="R128" t="s">
         <v>470</v>
@@ -18071,10 +18071,10 @@
         <v>406</v>
       </c>
       <c r="P129" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="Q129" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="R129" t="s">
         <v>470</v>
@@ -18187,7 +18187,7 @@
         <v>43</v>
       </c>
       <c r="Q130" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R130" t="s">
         <v>465</v>
@@ -18300,7 +18300,7 @@
         <v>43</v>
       </c>
       <c r="Q131" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R131" t="s">
         <v>465</v>
@@ -18413,7 +18413,7 @@
         <v>43</v>
       </c>
       <c r="Q132" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R132" t="s">
         <v>465</v>
@@ -18526,7 +18526,7 @@
         <v>43</v>
       </c>
       <c r="Q133" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R133" t="s">
         <v>465</v>
@@ -18639,7 +18639,7 @@
         <v>43</v>
       </c>
       <c r="Q134" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R134" t="s">
         <v>465</v>
@@ -18752,7 +18752,7 @@
         <v>43</v>
       </c>
       <c r="Q135" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R135" t="s">
         <v>465</v>
@@ -18865,7 +18865,7 @@
         <v>43</v>
       </c>
       <c r="Q136" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R136" t="s">
         <v>465</v>
@@ -18978,7 +18978,7 @@
         <v>43</v>
       </c>
       <c r="Q137" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="R137" t="s">
         <v>478</v>
@@ -19091,7 +19091,7 @@
         <v>43</v>
       </c>
       <c r="Q138" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R138" t="s">
         <v>465</v>
@@ -19204,7 +19204,7 @@
         <v>43</v>
       </c>
       <c r="Q139" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R139" t="s">
         <v>465</v>
@@ -19317,7 +19317,7 @@
         <v>43</v>
       </c>
       <c r="Q140" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R140" t="s">
         <v>465</v>
@@ -19430,7 +19430,7 @@
         <v>43</v>
       </c>
       <c r="Q141" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R141" t="s">
         <v>465</v>
@@ -19543,7 +19543,7 @@
         <v>43</v>
       </c>
       <c r="Q142" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R142" t="s">
         <v>465</v>
@@ -19656,7 +19656,7 @@
         <v>43</v>
       </c>
       <c r="Q143" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R143" t="s">
         <v>465</v>
@@ -19769,7 +19769,7 @@
         <v>43</v>
       </c>
       <c r="Q144" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R144" t="s">
         <v>465</v>
@@ -19882,7 +19882,7 @@
         <v>43</v>
       </c>
       <c r="Q145" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R145" t="s">
         <v>465</v>
@@ -19995,7 +19995,7 @@
         <v>43</v>
       </c>
       <c r="Q146" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R146" t="s">
         <v>465</v>
@@ -20108,7 +20108,7 @@
         <v>43</v>
       </c>
       <c r="Q147" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R147" t="s">
         <v>465</v>
@@ -20221,7 +20221,7 @@
         <v>43</v>
       </c>
       <c r="Q148" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R148" t="s">
         <v>465</v>
@@ -20334,7 +20334,7 @@
         <v>43</v>
       </c>
       <c r="Q149" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R149" t="s">
         <v>465</v>
@@ -20447,7 +20447,7 @@
         <v>43</v>
       </c>
       <c r="Q150" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R150" t="s">
         <v>465</v>
@@ -20560,7 +20560,7 @@
         <v>43</v>
       </c>
       <c r="Q151" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R151" t="s">
         <v>465</v>
@@ -20673,7 +20673,7 @@
         <v>43</v>
       </c>
       <c r="Q152" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R152" t="s">
         <v>465</v>
@@ -20786,7 +20786,7 @@
         <v>43</v>
       </c>
       <c r="Q153" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R153" t="s">
         <v>465</v>
@@ -20899,7 +20899,7 @@
         <v>43</v>
       </c>
       <c r="Q154" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R154" t="s">
         <v>465</v>
@@ -21012,7 +21012,7 @@
         <v>43</v>
       </c>
       <c r="Q155" t="s">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="R155" t="s">
         <v>465</v>
@@ -21125,7 +21125,7 @@
         <v>419</v>
       </c>
       <c r="Q156" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="R156" t="s">
         <v>479</v>
@@ -21238,7 +21238,7 @@
         <v>419</v>
       </c>
       <c r="Q157" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="R157" t="s">
         <v>479</v>
@@ -21351,7 +21351,7 @@
         <v>420</v>
       </c>
       <c r="Q158" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R158" t="s">
         <v>480</v>
@@ -21464,7 +21464,7 @@
         <v>420</v>
       </c>
       <c r="Q159" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R159" t="s">
         <v>480</v>
@@ -21577,7 +21577,7 @@
         <v>420</v>
       </c>
       <c r="Q160" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R160" t="s">
         <v>480</v>
@@ -21690,7 +21690,7 @@
         <v>420</v>
       </c>
       <c r="Q161" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R161" t="s">
         <v>480</v>
@@ -21803,7 +21803,7 @@
         <v>420</v>
       </c>
       <c r="Q162" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R162" t="s">
         <v>480</v>
@@ -21916,7 +21916,7 @@
         <v>420</v>
       </c>
       <c r="Q163" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R163" t="s">
         <v>480</v>
@@ -22026,10 +22026,10 @@
         <v>411</v>
       </c>
       <c r="P164" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q164" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R164" t="s">
         <v>481</v>
@@ -22136,13 +22136,13 @@
         <v>390</v>
       </c>
       <c r="O165" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="P165" t="s">
-        <v>43</v>
+        <v>420</v>
       </c>
       <c r="Q165" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="R165" t="s">
         <v>480</v>
@@ -22252,10 +22252,10 @@
         <v>411</v>
       </c>
       <c r="P166" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q166" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R166" t="s">
         <v>481</v>
@@ -22365,10 +22365,10 @@
         <v>411</v>
       </c>
       <c r="P167" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q167" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R167" t="s">
         <v>481</v>
@@ -22478,10 +22478,10 @@
         <v>411</v>
       </c>
       <c r="P168" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q168" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R168" t="s">
         <v>481</v>
@@ -22591,10 +22591,10 @@
         <v>411</v>
       </c>
       <c r="P169" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q169" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R169" t="s">
         <v>481</v>
@@ -22704,10 +22704,10 @@
         <v>411</v>
       </c>
       <c r="P170" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q170" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R170" t="s">
         <v>481</v>
@@ -22817,10 +22817,10 @@
         <v>411</v>
       </c>
       <c r="P171" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q171" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R171" t="s">
         <v>481</v>
@@ -22930,7 +22930,7 @@
         <v>411</v>
       </c>
       <c r="P172" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q172" t="s">
         <v>451</v>
@@ -23043,7 +23043,7 @@
         <v>411</v>
       </c>
       <c r="P173" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q173" t="s">
         <v>451</v>
@@ -23156,7 +23156,7 @@
         <v>411</v>
       </c>
       <c r="P174" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q174" t="s">
         <v>451</v>
@@ -23269,7 +23269,7 @@
         <v>411</v>
       </c>
       <c r="P175" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q175" t="s">
         <v>451</v>
@@ -23382,7 +23382,7 @@
         <v>411</v>
       </c>
       <c r="P176" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q176" t="s">
         <v>451</v>
@@ -23495,7 +23495,7 @@
         <v>411</v>
       </c>
       <c r="P177" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q177" t="s">
         <v>451</v>
@@ -23608,7 +23608,7 @@
         <v>411</v>
       </c>
       <c r="P178" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q178" t="s">
         <v>451</v>
@@ -23721,7 +23721,7 @@
         <v>411</v>
       </c>
       <c r="P179" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q179" t="s">
         <v>451</v>
@@ -23834,7 +23834,7 @@
         <v>411</v>
       </c>
       <c r="P180" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q180" t="s">
         <v>451</v>
@@ -23947,7 +23947,7 @@
         <v>411</v>
       </c>
       <c r="P181" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q181" t="s">
         <v>451</v>
@@ -24060,7 +24060,7 @@
         <v>411</v>
       </c>
       <c r="P182" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q182" t="s">
         <v>451</v>
@@ -24173,7 +24173,7 @@
         <v>411</v>
       </c>
       <c r="P183" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q183" t="s">
         <v>451</v>
@@ -24286,7 +24286,7 @@
         <v>411</v>
       </c>
       <c r="P184" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q184" t="s">
         <v>451</v>
@@ -24399,7 +24399,7 @@
         <v>411</v>
       </c>
       <c r="P185" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q185" t="s">
         <v>451</v>
@@ -24512,7 +24512,7 @@
         <v>411</v>
       </c>
       <c r="P186" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q186" t="s">
         <v>451</v>
@@ -24625,7 +24625,7 @@
         <v>411</v>
       </c>
       <c r="P187" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q187" t="s">
         <v>451</v>
@@ -24738,7 +24738,7 @@
         <v>411</v>
       </c>
       <c r="P188" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q188" t="s">
         <v>451</v>
@@ -24851,7 +24851,7 @@
         <v>411</v>
       </c>
       <c r="P189" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q189" t="s">
         <v>451</v>
@@ -24964,7 +24964,7 @@
         <v>411</v>
       </c>
       <c r="P190" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q190" t="s">
         <v>451</v>
@@ -25077,10 +25077,10 @@
         <v>411</v>
       </c>
       <c r="P191" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q191" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R191" t="s">
         <v>481</v>
@@ -25190,10 +25190,10 @@
         <v>411</v>
       </c>
       <c r="P192" t="s">
-        <v>43</v>
+        <v>421</v>
       </c>
       <c r="Q192" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="R192" t="s">
         <v>481</v>

</xml_diff>

<commit_message>
Remove periods at end of comparisons
Remove periods at end of comparisons so work in observation summary statements
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -1484,7 +1484,7 @@
     <t>10d vs 0d</t>
   </si>
   <si>
-    <t xml:space="preserve">positively correlated with antibody response at 28d &amp; onward. </t>
+    <t>positively correlated with antibody response at 28d &amp; onward</t>
   </si>
   <si>
     <t>1d vs 0d</t>
@@ -1562,7 +1562,7 @@
     <t>high vs low inositol phosphate metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines) </t>
+    <t>group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines)</t>
   </si>
   <si>
     <t>86d vs 0d</t>
@@ -1574,7 +1574,7 @@
     <t>S2 vs S1 as defined by hierarchical clustering of gene expression</t>
   </si>
   <si>
-    <t xml:space="preserve">S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response. </t>
+    <t>S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response</t>
   </si>
   <si>
     <t>3d vs 1d</t>

</xml_diff>

<commit_message>
Revert "Remove periods at end of comparisons"
This reverts commit fd0deaef2829674f141e742b9d76996fd5c4f7cc.
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -1484,7 +1484,7 @@
     <t>10d vs 0d</t>
   </si>
   <si>
-    <t>positively correlated with antibody response at 28d &amp; onward</t>
+    <t xml:space="preserve">positively correlated with antibody response at 28d &amp; onward. </t>
   </si>
   <si>
     <t>1d vs 0d</t>
@@ -1562,7 +1562,7 @@
     <t>high vs low inositol phosphate metabolism</t>
   </si>
   <si>
-    <t>group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines)</t>
+    <t xml:space="preserve">group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines) </t>
   </si>
   <si>
     <t>86d vs 0d</t>
@@ -1574,7 +1574,7 @@
     <t>S2 vs S1 as defined by hierarchical clustering of gene expression</t>
   </si>
   <si>
-    <t>S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response</t>
+    <t xml:space="preserve">S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response. </t>
   </si>
   <si>
     <t>3d vs 1d</t>

</xml_diff>

<commit_message>
Revert "Revert "Remove periods at end of comparisons""
This reverts commit ec263866490794252cd36c430bbae08b49a9929e.
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -1484,7 +1484,7 @@
     <t>10d vs 0d</t>
   </si>
   <si>
-    <t xml:space="preserve">positively correlated with antibody response at 28d &amp; onward. </t>
+    <t>positively correlated with antibody response at 28d &amp; onward</t>
   </si>
   <si>
     <t>1d vs 0d</t>
@@ -1562,7 +1562,7 @@
     <t>high vs low inositol phosphate metabolism</t>
   </si>
   <si>
-    <t xml:space="preserve">group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines) </t>
+    <t>group 2 (4mo: HBV &amp; OPV. 9mo: MV+DTP (i.m). 11mo: outstanding vaccines) vs groups 1 (4mo: 3rd dose of DTP, HBV, OPV. 9mo: 1 i.m dose of MV Edmonstron Zagreb strain. 11mo: outstanding vaccines) &amp; 3 (4mo: HBV &amp; OPV. 9mo: DTP. 11mo: outstanding vaccines)</t>
   </si>
   <si>
     <t>86d vs 0d</t>
@@ -1574,7 +1574,7 @@
     <t>S2 vs S1 as defined by hierarchical clustering of gene expression</t>
   </si>
   <si>
-    <t xml:space="preserve">S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response. </t>
+    <t>S2 vs S1 as defined by hierarchical clustering of gene expression. Both clusters d21/d0, where each cluster was enriched for a different vaccination route and different levels of antibody response</t>
   </si>
   <si>
     <t>3d vs 1d</t>

</xml_diff>

<commit_message>
update submissions after improve column descriptions
and change all ontology codes to use semicolon in type:code
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -671,7 +671,7 @@
     <t>skin of body</t>
   </si>
   <si>
-    <t>Cell Ontology ID</t>
+    <t>tissue cell ontology ID</t>
   </si>
   <si>
     <t>UBERON:0000178</t>
@@ -686,7 +686,7 @@
     <t>UBERON:0002097</t>
   </si>
   <si>
-    <t>response component (original cell type)</t>
+    <t>response component (original curated cell type)</t>
   </si>
   <si>
     <t>CD56-bright natural killer (NK) cells</t>
@@ -2183,130 +2183,130 @@
     <t>- roughly 60/40 female:male ratio, over 70% were Causasian</t>
   </si>
   <si>
-    <t>cell ontology ID</t>
-  </si>
-  <si>
-    <t>CL_0000946</t>
-  </si>
-  <si>
-    <t>CL_0000904</t>
-  </si>
-  <si>
-    <t>CL_0000900</t>
-  </si>
-  <si>
-    <t>CL_0000980</t>
-  </si>
-  <si>
-    <t>CL_0000623</t>
-  </si>
-  <si>
-    <t>CL_0000979</t>
-  </si>
-  <si>
-    <t>CL_0000782</t>
-  </si>
-  <si>
-    <t>CL_0000784</t>
-  </si>
-  <si>
-    <t>CL_0000084</t>
-  </si>
-  <si>
-    <t>CL_0000905</t>
-  </si>
-  <si>
-    <t>CL_0000236</t>
-  </si>
-  <si>
-    <t>CL_0002057</t>
-  </si>
-  <si>
-    <t>CL_0000792</t>
-  </si>
-  <si>
-    <t>CL_0000786</t>
-  </si>
-  <si>
-    <t>CL_0000624</t>
-  </si>
-  <si>
-    <t>CL_0000625</t>
-  </si>
-  <si>
-    <t>CL_0000738</t>
-  </si>
-  <si>
-    <t>CL_0000787</t>
-  </si>
-  <si>
-    <t>CL_0000982</t>
-  </si>
-  <si>
-    <t>CL_0000576</t>
-  </si>
-  <si>
-    <t>CL_0000897</t>
-  </si>
-  <si>
-    <t>CL_0000983</t>
-  </si>
-  <si>
-    <t>CL_0000984</t>
-  </si>
-  <si>
-    <t>CL_0000788</t>
-  </si>
-  <si>
-    <t>CL_0000939</t>
-  </si>
-  <si>
-    <t>CL_0002397</t>
-  </si>
-  <si>
-    <t>CL_0002396</t>
-  </si>
-  <si>
-    <t>CL_0000896</t>
-  </si>
-  <si>
-    <t>CL_0000775</t>
-  </si>
-  <si>
-    <t>CL_0000542</t>
-  </si>
-  <si>
-    <t>CL_0001054</t>
-  </si>
-  <si>
-    <t>CL_0000451</t>
-  </si>
-  <si>
-    <t>CL_0000815</t>
-  </si>
-  <si>
-    <t>CL_0000794</t>
-  </si>
-  <si>
-    <t>CL_0000798</t>
-  </si>
-  <si>
-    <t>CL_0001041</t>
-  </si>
-  <si>
-    <t>protein ontology ID</t>
+    <t>response component cell ontology ID</t>
+  </si>
+  <si>
+    <t>CL:0000946</t>
+  </si>
+  <si>
+    <t>CL:0000904</t>
+  </si>
+  <si>
+    <t>CL:0000900</t>
+  </si>
+  <si>
+    <t>CL:0000980</t>
+  </si>
+  <si>
+    <t>CL:0000623</t>
+  </si>
+  <si>
+    <t>CL:0000979</t>
+  </si>
+  <si>
+    <t>CL:0000782</t>
+  </si>
+  <si>
+    <t>CL:0000784</t>
+  </si>
+  <si>
+    <t>CL:0000084</t>
+  </si>
+  <si>
+    <t>CL:0000905</t>
+  </si>
+  <si>
+    <t>CL:0000236</t>
+  </si>
+  <si>
+    <t>CL:0002057</t>
+  </si>
+  <si>
+    <t>CL:0000792</t>
+  </si>
+  <si>
+    <t>CL:0000786</t>
+  </si>
+  <si>
+    <t>CL:0000624</t>
+  </si>
+  <si>
+    <t>CL:0000625</t>
+  </si>
+  <si>
+    <t>CL:0000738</t>
+  </si>
+  <si>
+    <t>CL:0000787</t>
+  </si>
+  <si>
+    <t>CL:0000982</t>
+  </si>
+  <si>
+    <t>CL:0000576</t>
+  </si>
+  <si>
+    <t>CL:0000897</t>
+  </si>
+  <si>
+    <t>CL:0000983</t>
+  </si>
+  <si>
+    <t>CL:0000984</t>
+  </si>
+  <si>
+    <t>CL:0000788</t>
+  </si>
+  <si>
+    <t>CL:0000939</t>
+  </si>
+  <si>
+    <t>CL:0002397</t>
+  </si>
+  <si>
+    <t>CL:0002396</t>
+  </si>
+  <si>
+    <t>CL:0000896</t>
+  </si>
+  <si>
+    <t>CL:0000775</t>
+  </si>
+  <si>
+    <t>CL:0000542</t>
+  </si>
+  <si>
+    <t>CL:0001054</t>
+  </si>
+  <si>
+    <t>CL:0000451</t>
+  </si>
+  <si>
+    <t>CL:0000815</t>
+  </si>
+  <si>
+    <t>CL:0000794</t>
+  </si>
+  <si>
+    <t>CL:0000798</t>
+  </si>
+  <si>
+    <t>CL:0001041</t>
+  </si>
+  <si>
+    <t>response component marker protein ontology ID</t>
   </si>
   <si>
     <t>PR:000001024</t>
   </si>
   <si>
-    <t>PR:000001020, PR_000001002, PR:000001963</t>
-  </si>
-  <si>
-    <t>PR_000001412</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR_P29965, PR_000001412 </t>
+    <t>PR:000001020, PR:000001002, PR:000001963</t>
+  </si>
+  <si>
+    <t>PR:000001412</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR:P29965, PR:000001412 </t>
   </si>
   <si>
     <t>PR:000000017</t>
@@ -2324,7 +2324,7 @@
     <t>PR:000001138</t>
   </si>
   <si>
-    <t xml:space="preserve">PR_Q96D21 </t>
+    <t xml:space="preserve">PR:Q96D21 </t>
   </si>
   <si>
     <t>PR:000001961</t>
@@ -2336,31 +2336,31 @@
     <t>PR:000001963, PR:000001408, PR:000001289</t>
   </si>
   <si>
-    <t xml:space="preserve">PR_000001383, PR_000025670 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">PR:000001963, PR_000001203 </t>
-  </si>
-  <si>
-    <t>PR_000001002, PR:000001963</t>
-  </si>
-  <si>
-    <t>PR_000001002, PR:000001963, PR:000001408</t>
-  </si>
-  <si>
-    <t>PR_000001483</t>
-  </si>
-  <si>
-    <t>PR_000001024, PR_000001483</t>
-  </si>
-  <si>
-    <t>PR:000001889, PR_000001483</t>
+    <t xml:space="preserve">PR:000001383, PR:000025670 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">PR:000001963, PR:000001203 </t>
+  </si>
+  <si>
+    <t>PR:000001002, PR:000001963</t>
+  </si>
+  <si>
+    <t>PR:000001002, PR:000001963, PR:000001408</t>
+  </si>
+  <si>
+    <t>PR:000001483</t>
+  </si>
+  <si>
+    <t>PR:000001024, PR:000001483</t>
+  </si>
+  <si>
+    <t>PR:000001889, PR:000001483</t>
   </si>
   <si>
     <t>PR:000001889, PR:000001289, PR:000001020</t>
   </si>
   <si>
-    <t>PR:000001020, PR_000001002, PR:000001289, PR:000001963</t>
+    <t>PR:000001020, PR:000001002, PR:000001289, PR:000001963</t>
   </si>
   <si>
     <t>PR:000001020, PR:000029630</t>
@@ -2372,7 +2372,7 @@
     <t>PR:000001865</t>
   </si>
   <si>
-    <t>PR:000001020, PR_000001002, PR:000001289</t>
+    <t>PR:000001020, PR:000001002, PR:000001289</t>
   </si>
   <si>
     <t>PR:000001013</t>
@@ -2387,19 +2387,19 @@
     <t>PR:000003499</t>
   </si>
   <si>
-    <t xml:space="preserve">PR_000001412 </t>
+    <t xml:space="preserve">PR:000001412 </t>
   </si>
   <si>
     <t>PR:000029630</t>
   </si>
   <si>
-    <t xml:space="preserve">PR_000001350 </t>
+    <t xml:space="preserve">PR:000001350 </t>
   </si>
   <si>
     <t>PR:000001020, PR:000001024</t>
   </si>
   <si>
-    <t xml:space="preserve">PR:000001379, PR_000002307 </t>
+    <t xml:space="preserve">PR:000001379, PR:000002307 </t>
   </si>
   <si>
     <t>PR:000001343</t>
@@ -2411,16 +2411,16 @@
     <t>PR:000002060, PR:000000017</t>
   </si>
   <si>
-    <t>PR_000001002, PR:000001343</t>
+    <t>PR:000001002, PR:000001343</t>
   </si>
   <si>
     <t>PR:000001467</t>
   </si>
   <si>
-    <t xml:space="preserve">PR_000001483, PR_000001024, PR:000001020 </t>
-  </si>
-  <si>
-    <t>PR_000001017, PR_000001203</t>
+    <t xml:space="preserve">PR:000001483, PR:000001024, PR:000001020 </t>
+  </si>
+  <si>
+    <t>PR:000001017, PR:000001203</t>
   </si>
   <si>
     <t>PR:000001963, PR:000001408</t>
@@ -2444,7 +2444,7 @@
     <t>response component count</t>
   </si>
   <si>
-    <t>ID of observation within its own submission</t>
+    <t xml:space="preserve">ID of observation within a publication (PMID) and for its submission type </t>
   </si>
   <si>
     <t>12</t>
@@ -2468,7 +2468,7 @@
     <t>24</t>
   </si>
   <si>
-    <t>Uniq ID of observation within its submission type</t>
+    <t>ID of observation within its submission type</t>
   </si>
   <si>
     <t>31</t>

</xml_diff>

<commit_message>
removed extraneous subgroup entries
</commit_message>
<xml_diff>
--- a/reformatted_data/cell_type-recreated_template.xlsx
+++ b/reformatted_data/cell_type-recreated_template.xlsx
@@ -767,7 +767,7 @@
     <t>influenza-specific IgA secreting plasmablasts</t>
   </si>
   <si>
-    <t>naive B cells (CD19-positive, IgD-negative, CD27-negative) (CL_0000788); memory B cells (CD19+, IgD-, CD27+) (CL_0001053); transitional B cells (CD19+, CD24+, CD38+) (CL_0000818)</t>
+    <t>naive B cells (CD19-positive, IgD-negative, CD27-negative) (CL:0000788); memory B cells (CD19+, IgD-, CD27+) (CL:0001053); transitional B cells (CD19+, CD24+, CD38+) (CL:0000818)</t>
   </si>
   <si>
     <t>plasmablasts (CD19+, CD27+, CD38+)</t>
@@ -1289,7 +1289,7 @@
     <t>MRKAd5/HIV</t>
   </si>
   <si>
-    <t>Modified Vaccinia Ankara (MVA) virus vaccine vector</t>
+    <t>modified Vaccinia Ankara (MVA) virus vaccine vector</t>
   </si>
   <si>
     <t>Menveo; ACWYVax</t>
@@ -1322,7 +1322,7 @@
     <t>FluMist</t>
   </si>
   <si>
-    <t>Inactivated influenza vaccine</t>
+    <t>inactivated influenza vaccine</t>
   </si>
   <si>
     <t>Measles virus vaccine; Diphtheria-Tetanus-Pertussis vaccine</t>
@@ -1535,7 +1535,7 @@
     <t>GLA-AF</t>
   </si>
   <si>
-    <t>AS03 (VO_0001320)</t>
+    <t>AS03 (VO:0001320)</t>
   </si>
   <si>
     <t>AS03 (GSK)</t>

</xml_diff>